<commit_message>
Distinguish between roles Student and GradStudent,
because Student cannot generate a prototype and a GradStudent can.
</commit_message>
<xml_diff>
--- a/RAP3/RAP3.xlsx
+++ b/RAP3/RAP3.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="228" windowWidth="11652" windowHeight="5340"/>
+    <workbookView xWindow="240" yWindow="225" windowWidth="11655" windowHeight="5340"/>
   </bookViews>
   <sheets>
     <sheet name="Identity Provider data" sheetId="2" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="51">
   <si>
     <t>Organization</t>
   </si>
@@ -164,6 +164,9 @@
   </si>
   <si>
     <t>debbiet</t>
+  </si>
+  <si>
+    <t>GradStudent</t>
   </si>
 </sst>
 </file>
@@ -270,9 +273,9 @@
     </xf>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Calculation" xfId="2" builtinId="22"/>
-    <cellStyle name="Neutral" xfId="1" builtinId="28"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Berekening" xfId="2" builtinId="22"/>
+    <cellStyle name="Neutraal" xfId="1" builtinId="28"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -285,9 +288,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Kantoor">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -325,7 +328,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Kantoor">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -397,7 +400,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Kantoor">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -574,22 +577,22 @@
   <dimension ref="A1:J18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.6640625" customWidth="1"/>
+    <col min="1" max="1" width="20.7109375" customWidth="1"/>
     <col min="2" max="2" width="15" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="19.109375" style="3" customWidth="1"/>
-    <col min="5" max="6" width="20.6640625" style="3" customWidth="1"/>
-    <col min="7" max="7" width="15.44140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.6640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.44140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.5546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="19.140625" style="3" customWidth="1"/>
+    <col min="5" max="6" width="20.7109375" style="3" customWidth="1"/>
+    <col min="7" max="7" width="15.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.5703125" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" s="1" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>14</v>
       </c>
@@ -609,7 +612,7 @@
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
     </row>
-    <row r="2" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" s="1" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
@@ -629,7 +632,7 @@
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="str">
         <f t="shared" ref="A3" si="0">IF($B3="","",CONCATENATE($B3," ",IF($C3="",D3,CONCATENATE($C3," ",$D3))))</f>
         <v>Stef Joosten</v>
@@ -641,7 +644,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A4" s="8" t="str">
         <f>IF($B4="","",CONCATENATE($B4," ",IF($C4="",D4,CONCATENATE($C4," ",$D4))))</f>
         <v>Lloyd Rutledge</v>
@@ -653,7 +656,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="str">
         <f t="shared" ref="A5:A6" si="1">IF($B5="","",CONCATENATE($B5," ",IF($C5="",D5,CONCATENATE($C5," ",$D5))))</f>
         <v>Rogier van der Wetering</v>
@@ -668,7 +671,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A6" s="8" t="str">
         <f t="shared" si="1"/>
         <v>Jan de Student</v>
@@ -683,7 +686,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A7" s="8" t="s">
         <v>39</v>
       </c>
@@ -694,7 +697,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" s="1" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>13</v>
       </c>
@@ -712,7 +715,7 @@
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
     </row>
-    <row r="9" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" s="1" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>0</v>
       </c>
@@ -730,7 +733,7 @@
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A10" s="8" t="str">
         <f>IF($B10="","",$B10)</f>
         <v>OUNL</v>
@@ -743,7 +746,7 @@
       </c>
       <c r="D10" s="4"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A11" s="8" t="s">
         <v>42</v>
       </c>
@@ -755,7 +758,7 @@
       </c>
       <c r="D11" s="4"/>
     </row>
-    <row r="12" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" s="1" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>1</v>
       </c>
@@ -785,7 +788,7 @@
       </c>
       <c r="J12" s="2"/>
     </row>
-    <row r="13" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" s="1" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>2</v>
       </c>
@@ -815,7 +818,7 @@
       </c>
       <c r="J13" s="2"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A14" s="7" t="str">
         <f>IF($B14="","",CONCATENATE("Acc_",$B3))</f>
         <v>Acc_Stef</v>
@@ -838,10 +841,10 @@
         <v>36</v>
       </c>
       <c r="I14" s="3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A15" s="7" t="str">
         <f t="shared" ref="A15:A18" si="2">IF($B15="","",CONCATENATE("Acc_",$B4))</f>
         <v>Acc_Lloyd</v>
@@ -857,14 +860,17 @@
         <v>Lloyd Rutledge</v>
       </c>
       <c r="E15" s="6" t="str">
-        <f t="shared" ref="E15:E18" si="4">$A$10</f>
+        <f t="shared" ref="E15:E17" si="4">$A$10</f>
         <v>OUNL</v>
       </c>
       <c r="G15" s="3" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="I15" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A16" s="7" t="str">
         <f t="shared" si="2"/>
         <v>Acc_Rogier</v>
@@ -890,7 +896,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="str">
         <f t="shared" si="2"/>
         <v>Acc_Jan</v>
@@ -916,7 +922,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="str">
         <f t="shared" si="2"/>
         <v>Acc_Debbie</v>
@@ -942,7 +948,7 @@
         <v>38</v>
       </c>
       <c r="I18" s="3" t="s">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="J18"/>
     </row>

</xml_diff>

<commit_message>
Add population for name[Role*RoleName][UNI,TOT]
</commit_message>
<xml_diff>
--- a/RAP3/RAP3.xlsx
+++ b/RAP3/RAP3.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="225" windowWidth="11655" windowHeight="5340"/>
+    <workbookView xWindow="240" yWindow="228" windowWidth="11652" windowHeight="5340"/>
   </bookViews>
   <sheets>
     <sheet name="Identity Provider data" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="145621" concurrentCalc="0"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="54">
   <si>
     <t>Organization</t>
   </si>
@@ -167,6 +167,15 @@
   </si>
   <si>
     <t>GradStudent</t>
+  </si>
+  <si>
+    <t>[Roles]</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>RoleName</t>
   </si>
 </sst>
 </file>
@@ -283,6 +292,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -330,7 +342,7 @@
     </a:clrScheme>
     <a:fontScheme name="Kantoor">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -365,7 +377,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -574,25 +586,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J18"/>
+  <dimension ref="A1:J24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.7109375" customWidth="1"/>
+    <col min="1" max="1" width="20.6640625" customWidth="1"/>
     <col min="2" max="2" width="15" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="19.140625" style="3" customWidth="1"/>
-    <col min="5" max="6" width="20.7109375" style="3" customWidth="1"/>
-    <col min="7" max="7" width="15.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="19.109375" style="3" customWidth="1"/>
+    <col min="5" max="6" width="20.6640625" style="3" customWidth="1"/>
+    <col min="7" max="7" width="15.44140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.44140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.5546875" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>14</v>
       </c>
@@ -612,7 +624,7 @@
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
     </row>
-    <row r="2" spans="1:10" s="1" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
@@ -632,7 +644,7 @@
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
     </row>
-    <row r="3" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="str">
         <f t="shared" ref="A3" si="0">IF($B3="","",CONCATENATE($B3," ",IF($C3="",D3,CONCATENATE($C3," ",$D3))))</f>
         <v>Stef Joosten</v>
@@ -644,7 +656,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="8" t="str">
         <f>IF($B4="","",CONCATENATE($B4," ",IF($C4="",D4,CONCATENATE($C4," ",$D4))))</f>
         <v>Lloyd Rutledge</v>
@@ -656,7 +668,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="str">
         <f t="shared" ref="A5:A6" si="1">IF($B5="","",CONCATENATE($B5," ",IF($C5="",D5,CONCATENATE($C5," ",$D5))))</f>
         <v>Rogier van der Wetering</v>
@@ -671,7 +683,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="8" t="str">
         <f t="shared" si="1"/>
         <v>Jan de Student</v>
@@ -686,7 +698,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="8" t="s">
         <v>39</v>
       </c>
@@ -697,7 +709,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="1:10" s="1" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>13</v>
       </c>
@@ -715,7 +727,7 @@
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
     </row>
-    <row r="9" spans="1:10" s="1" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>0</v>
       </c>
@@ -733,7 +745,7 @@
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
     </row>
-    <row r="10" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="8" t="str">
         <f>IF($B10="","",$B10)</f>
         <v>OUNL</v>
@@ -746,7 +758,7 @@
       </c>
       <c r="D10" s="4"/>
     </row>
-    <row r="11" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="8" t="s">
         <v>42</v>
       </c>
@@ -758,7 +770,7 @@
       </c>
       <c r="D11" s="4"/>
     </row>
-    <row r="12" spans="1:10" s="1" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>1</v>
       </c>
@@ -788,7 +800,7 @@
       </c>
       <c r="J12" s="2"/>
     </row>
-    <row r="13" spans="1:10" s="1" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>2</v>
       </c>
@@ -818,7 +830,7 @@
       </c>
       <c r="J13" s="2"/>
     </row>
-    <row r="14" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" s="7" t="str">
         <f>IF($B14="","",CONCATENATE("Acc_",$B3))</f>
         <v>Acc_Stef</v>
@@ -844,7 +856,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" s="7" t="str">
         <f t="shared" ref="A15:A18" si="2">IF($B15="","",CONCATENATE("Acc_",$B4))</f>
         <v>Acc_Lloyd</v>
@@ -870,7 +882,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" s="7" t="str">
         <f t="shared" si="2"/>
         <v>Acc_Rogier</v>
@@ -896,7 +908,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="str">
         <f t="shared" si="2"/>
         <v>Acc_Jan</v>
@@ -922,7 +934,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" s="7" t="str">
         <f t="shared" si="2"/>
         <v>Acc_Debbie</v>
@@ -951,6 +963,54 @@
         <v>50</v>
       </c>
       <c r="J18"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>36</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>35</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>50</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>38</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>38</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
RAP3 - updated for better student registration/login. Some modifications to scripting interface layout.
</commit_message>
<xml_diff>
--- a/RAP3/RAP3.xlsx
+++ b/RAP3/RAP3.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="228" windowWidth="11652" windowHeight="5340"/>
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="Identity Provider data" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511" concurrentCalc="0"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
 </workbook>
 </file>
 
@@ -148,9 +148,6 @@
     <t>Hogeschool Arnhem Nijmegen</t>
   </si>
   <si>
-    <t>studentnummer</t>
-  </si>
-  <si>
     <t>Studentnummer</t>
   </si>
   <si>
@@ -176,6 +173,9 @@
   </si>
   <si>
     <t>RoleName</t>
+  </si>
+  <si>
+    <t>accStudNr</t>
   </si>
 </sst>
 </file>
@@ -282,9 +282,9 @@
     </xf>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Berekening" xfId="2" builtinId="22"/>
-    <cellStyle name="Neutraal" xfId="1" builtinId="28"/>
-    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+    <cellStyle name="Calculation" xfId="2" builtinId="22"/>
+    <cellStyle name="Neutral" xfId="1" builtinId="28"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -300,9 +300,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Kantoor">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -340,9 +340,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Kantoor">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -377,7 +377,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -412,7 +412,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Kantoor">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -589,7 +589,7 @@
   <dimension ref="A1:J24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -787,7 +787,7 @@
         <v>22</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="G12" s="2" t="s">
         <v>20</v>
@@ -817,7 +817,7 @@
         <v>0</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G13" s="2" t="s">
         <v>8</v>
@@ -836,7 +836,7 @@
         <v>Acc_Stef</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>24</v>
@@ -853,7 +853,7 @@
         <v>36</v>
       </c>
       <c r="I14" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
@@ -862,7 +862,7 @@
         <v>Acc_Lloyd</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>24</v>
@@ -879,7 +879,7 @@
         <v>36</v>
       </c>
       <c r="I15" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
@@ -888,7 +888,7 @@
         <v>Acc_Rogier</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>24</v>
@@ -940,7 +940,7 @@
         <v>Acc_Debbie</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C18" s="9" t="s">
         <v>24</v>
@@ -960,16 +960,16 @@
         <v>38</v>
       </c>
       <c r="I18" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J18"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B19" s="2" t="s">
         <v>51</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.3">
@@ -977,7 +977,7 @@
         <v>8</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.3">
@@ -998,10 +998,10 @@
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
preparing for install of RAP3 on Azure
</commit_message>
<xml_diff>
--- a/RAP3/RAP3.xlsx
+++ b/RAP3/RAP3.xlsx
@@ -4,17 +4,17 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="228" windowWidth="11652" windowHeight="5340"/>
+    <workbookView xWindow="240" yWindow="225" windowWidth="11655" windowHeight="5340"/>
   </bookViews>
   <sheets>
     <sheet name="Identity Provider data" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="145621" concurrentCalc="0"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="52">
   <si>
     <t>Organization</t>
   </si>
@@ -61,16 +61,10 @@
     <t>[PersonReg]</t>
   </si>
   <si>
-    <t>OrgAbbrName</t>
-  </si>
-  <si>
     <t>orgAbbrName</t>
   </si>
   <si>
     <t>orgFullName</t>
-  </si>
-  <si>
-    <t>OrgFullName</t>
   </si>
   <si>
     <t>Joosten</t>
@@ -282,9 +276,9 @@
     </xf>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Calculation" xfId="2" builtinId="22"/>
-    <cellStyle name="Neutral" xfId="1" builtinId="28"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Berekening" xfId="2" builtinId="22"/>
+    <cellStyle name="Neutraal" xfId="1" builtinId="28"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -300,9 +294,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Kantoor">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -340,7 +334,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Kantoor">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -412,7 +406,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Kantoor">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -589,22 +583,22 @@
   <dimension ref="A1:J24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.6640625" customWidth="1"/>
+    <col min="1" max="1" width="20.7109375" customWidth="1"/>
     <col min="2" max="2" width="15" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="19.109375" style="3" customWidth="1"/>
-    <col min="5" max="6" width="20.6640625" style="3" customWidth="1"/>
-    <col min="7" max="7" width="15.44140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.6640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.44140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.5546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="19.140625" style="3" customWidth="1"/>
+    <col min="5" max="6" width="20.7109375" style="3" customWidth="1"/>
+    <col min="7" max="7" width="15.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.5703125" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" s="1" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>14</v>
       </c>
@@ -612,7 +606,7 @@
         <v>9</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>12</v>
@@ -624,7 +618,7 @@
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
     </row>
-    <row r="2" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" s="1" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
@@ -632,7 +626,7 @@
         <v>10</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>11</v>
@@ -644,80 +638,80 @@
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="str">
         <f t="shared" ref="A3" si="0">IF($B3="","",CONCATENATE($B3," ",IF($C3="",D3,CONCATENATE($C3," ",$D3))))</f>
         <v>Stef Joosten</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A4" s="8" t="str">
         <f>IF($B4="","",CONCATENATE($B4," ",IF($C4="",D4,CONCATENATE($C4," ",$D4))))</f>
         <v>Lloyd Rutledge</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="str">
         <f t="shared" ref="A5:A6" si="1">IF($B5="","",CONCATENATE($B5," ",IF($C5="",D5,CONCATENATE($C5," ",$D5))))</f>
         <v>Rogier van der Wetering</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A6" s="8" t="str">
         <f t="shared" si="1"/>
         <v>Jan de Student</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C6" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A7" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="D6" s="3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A7" s="8" t="s">
+      <c r="B7" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D7" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="B7" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="1:10" s="1" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B8" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>16</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>17</v>
       </c>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
@@ -727,16 +721,12 @@
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
     </row>
-    <row r="9" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" s="1" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B9" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>18</v>
-      </c>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
@@ -745,32 +735,32 @@
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A10" s="8" t="str">
         <f>IF($B10="","",$B10)</f>
         <v>OUNL</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D10" s="4"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A11" s="8" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D11" s="4"/>
     </row>
-    <row r="12" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" s="1" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>1</v>
       </c>
@@ -781,26 +771,26 @@
         <v>4</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="J12" s="2"/>
     </row>
-    <row r="13" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" s="1" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>2</v>
       </c>
@@ -813,11 +803,9 @@
       <c r="D13" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E13" s="2" t="s">
-        <v>0</v>
-      </c>
+      <c r="E13" s="2"/>
       <c r="F13" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G13" s="2" t="s">
         <v>8</v>
@@ -830,16 +818,16 @@
       </c>
       <c r="J13" s="2"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A14" s="7" t="str">
         <f>IF($B14="","",CONCATENATE("Acc_",$B3))</f>
         <v>Acc_Stef</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D14" s="6" t="str">
         <f>$A3</f>
@@ -850,22 +838,22 @@
         <v>OUNL</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="I14" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A15" s="7" t="str">
         <f t="shared" ref="A15:A18" si="2">IF($B15="","",CONCATENATE("Acc_",$B4))</f>
         <v>Acc_Lloyd</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D15" s="6" t="str">
         <f t="shared" ref="D15" si="3">$A4</f>
@@ -876,22 +864,22 @@
         <v>OUNL</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="I15" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A16" s="7" t="str">
         <f t="shared" si="2"/>
         <v>Acc_Rogier</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D16" s="6" t="str">
         <f t="shared" ref="D16" si="5">$A5</f>
@@ -902,13 +890,13 @@
         <v>OUNL</v>
       </c>
       <c r="G16" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="H16" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="H16" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="17" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="str">
         <f t="shared" si="2"/>
         <v>Acc_Jan</v>
@@ -917,7 +905,7 @@
         <v>123456</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D17" s="6" t="str">
         <f>$A6</f>
@@ -931,22 +919,22 @@
         <v>123456</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="str">
         <f t="shared" si="2"/>
         <v>Acc_Debbie</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E18" s="6" t="str">
         <f>$A$11</f>
@@ -954,62 +942,62 @@
       </c>
       <c r="F18"/>
       <c r="G18" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="H18" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="H18" s="3" t="s">
-        <v>38</v>
-      </c>
       <c r="I18" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="J18"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B19" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="J18"/>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A19" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>34</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>33</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>47</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>36</v>
       </c>
-      <c r="B21" s="5" t="s">
+      <c r="B24" s="5" t="s">
         <v>36</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>35</v>
-      </c>
-      <c r="B22" s="5" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
-        <v>49</v>
-      </c>
-      <c r="B23" s="5" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
-        <v>38</v>
-      </c>
-      <c r="B24" s="5" t="s">
-        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add population for accIsActive[Account*Account]
</commit_message>
<xml_diff>
--- a/RAP3/RAP3.xlsx
+++ b/RAP3/RAP3.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="225" windowWidth="11655" windowHeight="5340"/>
+    <workbookView xWindow="240" yWindow="228" windowWidth="11652" windowHeight="5340"/>
   </bookViews>
   <sheets>
     <sheet name="Identity Provider data" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="53">
   <si>
     <t>Organization</t>
   </si>
@@ -170,6 +170,9 @@
   </si>
   <si>
     <t>accStudNr</t>
+  </si>
+  <si>
+    <t>accIsActive</t>
   </si>
 </sst>
 </file>
@@ -336,7 +339,7 @@
     </a:clrScheme>
     <a:fontScheme name="Kantoor">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -371,7 +374,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -583,22 +586,22 @@
   <dimension ref="A1:J24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.7109375" customWidth="1"/>
+    <col min="1" max="1" width="20.6640625" customWidth="1"/>
     <col min="2" max="2" width="15" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="19.140625" style="3" customWidth="1"/>
-    <col min="5" max="6" width="20.7109375" style="3" customWidth="1"/>
-    <col min="7" max="7" width="15.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="19.109375" style="3" customWidth="1"/>
+    <col min="5" max="6" width="20.6640625" style="3" customWidth="1"/>
+    <col min="7" max="7" width="15.44140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.44140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.5546875" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>14</v>
       </c>
@@ -618,7 +621,7 @@
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
     </row>
-    <row r="2" spans="1:10" s="1" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
@@ -638,7 +641,7 @@
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
     </row>
-    <row r="3" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="str">
         <f t="shared" ref="A3" si="0">IF($B3="","",CONCATENATE($B3," ",IF($C3="",D3,CONCATENATE($C3," ",$D3))))</f>
         <v>Stef Joosten</v>
@@ -650,7 +653,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="8" t="str">
         <f>IF($B4="","",CONCATENATE($B4," ",IF($C4="",D4,CONCATENATE($C4," ",$D4))))</f>
         <v>Lloyd Rutledge</v>
@@ -662,7 +665,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="str">
         <f t="shared" ref="A5:A6" si="1">IF($B5="","",CONCATENATE($B5," ",IF($C5="",D5,CONCATENATE($C5," ",$D5))))</f>
         <v>Rogier van der Wetering</v>
@@ -677,7 +680,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="8" t="str">
         <f t="shared" si="1"/>
         <v>Jan de Student</v>
@@ -692,7 +695,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="8" t="s">
         <v>37</v>
       </c>
@@ -703,7 +706,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="8" spans="1:10" s="1" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>13</v>
       </c>
@@ -721,7 +724,7 @@
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
     </row>
-    <row r="9" spans="1:10" s="1" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>0</v>
       </c>
@@ -735,7 +738,7 @@
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
     </row>
-    <row r="10" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="8" t="str">
         <f>IF($B10="","",$B10)</f>
         <v>OUNL</v>
@@ -748,7 +751,7 @@
       </c>
       <c r="D10" s="4"/>
     </row>
-    <row r="11" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="8" t="s">
         <v>40</v>
       </c>
@@ -760,7 +763,7 @@
       </c>
       <c r="D11" s="4"/>
     </row>
-    <row r="12" spans="1:10" s="1" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>1</v>
       </c>
@@ -788,9 +791,11 @@
       <c r="I12" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="J12" s="2"/>
-    </row>
-    <row r="13" spans="1:10" s="1" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="J12" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>2</v>
       </c>
@@ -816,9 +821,11 @@
       <c r="I13" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J13" s="2"/>
-    </row>
-    <row r="14" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="J13" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" s="7" t="str">
         <f>IF($B14="","",CONCATENATE("Acc_",$B3))</f>
         <v>Acc_Stef</v>
@@ -840,11 +847,18 @@
       <c r="G14" s="3" t="s">
         <v>34</v>
       </c>
+      <c r="H14" s="3" t="s">
+        <v>36</v>
+      </c>
       <c r="I14" s="3" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="J14" s="3" t="str">
+        <f>A14</f>
+        <v>Acc_Stef</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" s="7" t="str">
         <f t="shared" ref="A15:A18" si="2">IF($B15="","",CONCATENATE("Acc_",$B4))</f>
         <v>Acc_Lloyd</v>
@@ -869,8 +883,12 @@
       <c r="I15" s="3" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="J15" s="3" t="str">
+        <f t="shared" ref="J15:J18" si="5">A15</f>
+        <v>Acc_Lloyd</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" s="7" t="str">
         <f t="shared" si="2"/>
         <v>Acc_Rogier</v>
@@ -882,7 +900,7 @@
         <v>22</v>
       </c>
       <c r="D16" s="6" t="str">
-        <f t="shared" ref="D16" si="5">$A5</f>
+        <f t="shared" ref="D16" si="6">$A5</f>
         <v>Rogier van der Wetering</v>
       </c>
       <c r="E16" s="6" t="str">
@@ -895,8 +913,12 @@
       <c r="H16" s="3" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="J16" s="3" t="str">
+        <f t="shared" si="5"/>
+        <v>Acc_Rogier</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="str">
         <f t="shared" si="2"/>
         <v>Acc_Jan</v>
@@ -921,8 +943,12 @@
       <c r="G17" s="3" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J17" s="3" t="str">
+        <f t="shared" si="5"/>
+        <v>Acc_Jan</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" s="7" t="str">
         <f t="shared" si="2"/>
         <v>Acc_Debbie</v>
@@ -950,9 +976,12 @@
       <c r="I18" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="J18"/>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J18" s="3" t="str">
+        <f t="shared" si="5"/>
+        <v>Acc_Debbie</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>48</v>
       </c>
@@ -960,7 +989,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>8</v>
       </c>
@@ -968,7 +997,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>34</v>
       </c>
@@ -976,7 +1005,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>33</v>
       </c>
@@ -984,7 +1013,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>47</v>
       </c>
@@ -992,7 +1021,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>36</v>
       </c>

</xml_diff>

<commit_message>
Added extra Student accounts in initial population
</commit_message>
<xml_diff>
--- a/RAP3/RAP3.xlsx
+++ b/RAP3/RAP3.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="80">
   <si>
     <t>Organization</t>
   </si>
@@ -173,6 +173,87 @@
   </si>
   <si>
     <t>accIsActive</t>
+  </si>
+  <si>
+    <t>S1</t>
+  </si>
+  <si>
+    <t>S2</t>
+  </si>
+  <si>
+    <t>S3</t>
+  </si>
+  <si>
+    <t>S4</t>
+  </si>
+  <si>
+    <t>S5</t>
+  </si>
+  <si>
+    <t>S6</t>
+  </si>
+  <si>
+    <t>S7</t>
+  </si>
+  <si>
+    <t>S8</t>
+  </si>
+  <si>
+    <t>S9</t>
+  </si>
+  <si>
+    <t>S10</t>
+  </si>
+  <si>
+    <t>S11</t>
+  </si>
+  <si>
+    <t>S12</t>
+  </si>
+  <si>
+    <t>Tudent</t>
+  </si>
+  <si>
+    <t>Ordina</t>
+  </si>
+  <si>
+    <t>ORD</t>
+  </si>
+  <si>
+    <t>Acc_S1</t>
+  </si>
+  <si>
+    <t>Acc_S2</t>
+  </si>
+  <si>
+    <t>Acc_S3</t>
+  </si>
+  <si>
+    <t>Acc_S4</t>
+  </si>
+  <si>
+    <t>Acc_S5</t>
+  </si>
+  <si>
+    <t>Acc_S6</t>
+  </si>
+  <si>
+    <t>Acc_S7</t>
+  </si>
+  <si>
+    <t>Acc_S8</t>
+  </si>
+  <si>
+    <t>Acc_S9</t>
+  </si>
+  <si>
+    <t>Acc_S10</t>
+  </si>
+  <si>
+    <t>Acc_S11</t>
+  </si>
+  <si>
+    <t>Acc_S12</t>
   </si>
 </sst>
 </file>
@@ -583,10 +664,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J24"/>
+  <dimension ref="A1:J49"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+      <selection activeCell="I31" sqref="I31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -667,7 +748,7 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="str">
-        <f t="shared" ref="A5:A6" si="1">IF($B5="","",CONCATENATE($B5," ",IF($C5="",D5,CONCATENATE($C5," ",$D5))))</f>
+        <f t="shared" ref="A5:A18" si="1">IF($B5="","",CONCATENATE($B5," ",IF($C5="",D5,CONCATENATE($C5," ",$D5))))</f>
         <v>Rogier van der Wetering</v>
       </c>
       <c r="B5" s="5" t="s">
@@ -681,351 +762,819 @@
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A6" s="8" t="str">
+      <c r="A6" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A7" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A8" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A9" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A10" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A11" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A12" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A13" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A14" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A15" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A16" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A17" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A18" s="8" t="str">
         <f t="shared" si="1"/>
         <v>Jan de Student</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B18" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C18" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D18" s="3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A7" s="8" t="s">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A19" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B19" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D19" s="3" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="8" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
+    <row r="20" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B20" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C20" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
-      <c r="J8" s="2"/>
-    </row>
-    <row r="9" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+      <c r="G20" s="2"/>
+      <c r="H20" s="2"/>
+      <c r="I20" s="2"/>
+      <c r="J20" s="2"/>
+    </row>
+    <row r="21" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
-      <c r="J9" s="2"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A10" s="8" t="str">
-        <f>IF($B10="","",$B10)</f>
+      <c r="B21" s="2"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="2"/>
+      <c r="H21" s="2"/>
+      <c r="I21" s="2"/>
+      <c r="J21" s="2"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A22" s="8" t="str">
+        <f>IF($B22="","",$B22)</f>
         <v>OUNL</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B22" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C22" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="D10" s="4"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A11" s="8" t="s">
+      <c r="D22" s="4"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A23" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="D23" s="4"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A24" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B24" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C24" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="D11" s="4"/>
-    </row>
-    <row r="12" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="1" t="s">
+      <c r="D24" s="4"/>
+    </row>
+    <row r="25" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B25" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C25" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="D25" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="E12" s="2" t="s">
+      <c r="E25" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="F12" s="2" t="s">
+      <c r="F25" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="G12" s="2" t="s">
+      <c r="G25" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="H12" s="2" t="s">
+      <c r="H25" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="I12" s="2" t="s">
+      <c r="I25" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="J12" s="2" t="s">
+      <c r="J25" s="2" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="13" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="1" t="s">
+    <row r="26" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B26" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C26" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="D26" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2" t="s">
+      <c r="E26" s="2"/>
+      <c r="F26" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="G13" s="2" t="s">
+      <c r="G26" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H13" s="2" t="s">
+      <c r="H26" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="I13" s="2" t="s">
+      <c r="I26" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J13" s="2" t="s">
+      <c r="J26" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A14" s="7" t="str">
-        <f>IF($B14="","",CONCATENATE("Acc_",$B3))</f>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A27" s="7" t="str">
+        <f>IF($B27="","",CONCATENATE("Acc_",$B3))</f>
         <v>Acc_Stef</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="B27" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="C14" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D14" s="6" t="str">
+      <c r="C27" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D27" s="6" t="str">
         <f>$A3</f>
         <v>Stef Joosten</v>
       </c>
-      <c r="E14" s="6" t="str">
-        <f>$A$10</f>
+      <c r="E27" s="6" t="str">
+        <f>$A$22</f>
         <v>OUNL</v>
       </c>
-      <c r="G14" s="3" t="s">
+      <c r="G27" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="H14" s="3" t="s">
+      <c r="H27" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="I14" s="3" t="s">
+      <c r="I27" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="J14" s="3" t="str">
-        <f>A14</f>
+      <c r="J27" s="3" t="str">
+        <f>A27</f>
         <v>Acc_Stef</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A15" s="7" t="str">
-        <f t="shared" ref="A15:A18" si="2">IF($B15="","",CONCATENATE("Acc_",$B4))</f>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A28" s="7" t="str">
+        <f>IF($B28="","",CONCATENATE("Acc_",$B4))</f>
         <v>Acc_Lloyd</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="B28" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="C15" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D15" s="6" t="str">
-        <f t="shared" ref="D15" si="3">$A4</f>
+      <c r="C28" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D28" s="6" t="str">
+        <f>$A4</f>
         <v>Lloyd Rutledge</v>
       </c>
-      <c r="E15" s="6" t="str">
-        <f t="shared" ref="E15:E17" si="4">$A$10</f>
+      <c r="E28" s="6" t="str">
+        <f t="shared" ref="E28:E30" si="2">$A$22</f>
         <v>OUNL</v>
       </c>
-      <c r="G15" s="3" t="s">
+      <c r="G28" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="I15" s="3" t="s">
+      <c r="I28" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="J15" s="3" t="str">
-        <f t="shared" ref="J15:J18" si="5">A15</f>
+      <c r="J28" s="3" t="str">
+        <f t="shared" ref="J28:J43" si="3">A28</f>
         <v>Acc_Lloyd</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A16" s="7" t="str">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A29" s="7" t="str">
+        <f>IF($B29="","",CONCATENATE("Acc_",$B5))</f>
+        <v>Acc_Rogier</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D29" s="6" t="str">
+        <f t="shared" ref="D29" si="4">$A5</f>
+        <v>Rogier van der Wetering</v>
+      </c>
+      <c r="E29" s="6" t="str">
         <f t="shared" si="2"/>
+        <v>OUNL</v>
+      </c>
+      <c r="G29" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="H29" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="J29" s="3" t="str">
+        <f t="shared" si="3"/>
         <v>Acc_Rogier</v>
       </c>
-      <c r="B16" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D16" s="6" t="str">
-        <f t="shared" ref="D16" si="6">$A5</f>
-        <v>Rogier van der Wetering</v>
-      </c>
-      <c r="E16" s="6" t="str">
-        <f t="shared" si="4"/>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A30" s="7" t="str">
+        <f>IF($B30="","",CONCATENATE("Acc_",$B18))</f>
+        <v>Acc_Jan</v>
+      </c>
+      <c r="B30" s="5">
+        <v>123456</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D30" s="6" t="str">
+        <f>$A18</f>
+        <v>Jan de Student</v>
+      </c>
+      <c r="E30" s="6" t="str">
+        <f t="shared" si="2"/>
         <v>OUNL</v>
       </c>
-      <c r="G16" s="3" t="s">
+      <c r="F30" s="3">
+        <v>123456</v>
+      </c>
+      <c r="G30" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="J30" s="3" t="str">
+        <f t="shared" si="3"/>
+        <v>Acc_Jan</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A31" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D31" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="E31" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="F31" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="G31" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="J31" s="3" t="str">
+        <f t="shared" si="3"/>
+        <v>Acc_S1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A32" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D32" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="E32" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="F32" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="G32" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="J32" s="3" t="str">
+        <f t="shared" si="3"/>
+        <v>Acc_S2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A33" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D33" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="E33" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="F33" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="G33" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="J33" s="3" t="str">
+        <f t="shared" si="3"/>
+        <v>Acc_S3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A34" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D34" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="E34" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="F34" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="G34" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="J34" s="3" t="str">
+        <f t="shared" si="3"/>
+        <v>Acc_S4</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A35" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D35" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="E35" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="F35" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="G35" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="J35" s="3" t="str">
+        <f t="shared" si="3"/>
+        <v>Acc_S5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A36" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D36" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="E36" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="F36" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="G36" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="J36" s="3" t="str">
+        <f t="shared" si="3"/>
+        <v>Acc_S6</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A37" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D37" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="E37" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="F37" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="G37" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="J37" s="3" t="str">
+        <f t="shared" si="3"/>
+        <v>Acc_S7</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A38" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D38" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="E38" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="F38" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="G38" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="J38" s="3" t="str">
+        <f t="shared" si="3"/>
+        <v>Acc_S8</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A39" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D39" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="E39" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="F39" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="G39" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="J39" s="3" t="str">
+        <f t="shared" si="3"/>
+        <v>Acc_S9</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A40" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="B40" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D40" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="E40" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="F40" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="G40" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="J40" s="3" t="str">
+        <f t="shared" si="3"/>
+        <v>Acc_S10</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A41" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="B41" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D41" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="E41" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="F41" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="G41" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="J41" s="3" t="str">
+        <f t="shared" si="3"/>
+        <v>Acc_S11</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A42" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="B42" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D42" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="E42" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="F42" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="G42" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="J42" s="3" t="str">
+        <f t="shared" si="3"/>
+        <v>Acc_S12</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A43" s="7" t="str">
+        <f>IF($B43="","",CONCATENATE("Acc_",$B19))</f>
+        <v>Acc_Debbie</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C43" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D43" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="E43" s="6" t="str">
+        <f>$A$24</f>
+        <v>HAN</v>
+      </c>
+      <c r="F43"/>
+      <c r="G43" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="H16" s="3" t="s">
+      <c r="H43" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="J16" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v>Acc_Rogier</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A17" s="7" t="str">
-        <f t="shared" si="2"/>
-        <v>Acc_Jan</v>
-      </c>
-      <c r="B17" s="5">
-        <v>123456</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D17" s="6" t="str">
-        <f>$A6</f>
-        <v>Jan de Student</v>
-      </c>
-      <c r="E17" s="6" t="str">
-        <f t="shared" si="4"/>
-        <v>OUNL</v>
-      </c>
-      <c r="F17" s="3">
-        <v>123456</v>
-      </c>
-      <c r="G17" s="3" t="s">
+      <c r="I43" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="J43" s="3" t="str">
+        <f t="shared" si="3"/>
+        <v>Acc_Debbie</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A44" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A45" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>34</v>
+      </c>
+      <c r="B46" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
         <v>33</v>
       </c>
-      <c r="J17" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v>Acc_Jan</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A18" s="7" t="str">
-        <f t="shared" si="2"/>
-        <v>Acc_Debbie</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="C18" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="D18" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="E18" s="6" t="str">
-        <f>$A$11</f>
-        <v>HAN</v>
-      </c>
-      <c r="F18"/>
-      <c r="G18" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="H18" s="3" t="s">
+      <c r="B47" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>47</v>
+      </c>
+      <c r="B48" s="5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
         <v>36</v>
       </c>
-      <c r="I18" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="J18" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v>Acc_Debbie</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A19" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A20" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
-        <v>34</v>
-      </c>
-      <c r="B21" s="5" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>33</v>
-      </c>
-      <c r="B22" s="5" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
-        <v>47</v>
-      </c>
-      <c r="B23" s="5" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
-        <v>36</v>
-      </c>
-      <c r="B24" s="5" t="s">
+      <c r="B49" s="5" t="s">
         <v>36</v>
       </c>
     </row>

</xml_diff>